<commit_message>
[FIX] budget overview report
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_all_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_all_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">Budget All Report</t>
   </si>
@@ -34,6 +34,30 @@
     <t xml:space="preserve">Budget</t>
   </si>
   <si>
+    <t xml:space="preserve">Charge Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget Method</t>
+  </si>
+  <si>
     <t xml:space="preserve">Run By</t>
   </si>
   <si>
@@ -47,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Activity Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge Type</t>
   </si>
   <si>
     <t xml:space="preserve">Activity</t>
@@ -296,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,73 +359,108 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" s="8" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="7" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="7" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="7" t="s">
+    </row>
+    <row r="17" s="8" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="D17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="J17" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>